<commit_message>
Changed to allow export to HDL
</commit_message>
<xml_diff>
--- a/docs/sinais.xlsx
+++ b/docs/sinais.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\8BitCPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\CpuDidatica\CpuDidatica\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC728AA-580A-4270-B2CD-F0D5AEC36FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49FDAC5-1B06-426F-BDE4-3FBC4196E9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1290" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{18A684C2-09AA-4094-803A-4CBD9ADAA45C}"/>
+    <workbookView xWindow="-20610" yWindow="1290" windowWidth="20730" windowHeight="11310" xr2:uid="{18A684C2-09AA-4094-803A-4CBD9ADAA45C}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções" sheetId="1" r:id="rId1"/>
-    <sheet name="ALU" sheetId="2" r:id="rId2"/>
+    <sheet name="Sinais" sheetId="3" r:id="rId2"/>
+    <sheet name="ALU" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="115">
   <si>
     <t>ROM</t>
   </si>
@@ -46,18 +47,12 @@
     <t>NOP</t>
   </si>
   <si>
-    <t>LDROM</t>
-  </si>
-  <si>
     <t>AE</t>
   </si>
   <si>
     <t>IRZ</t>
   </si>
   <si>
-    <t>MUX</t>
-  </si>
-  <si>
     <t>OP0</t>
   </si>
   <si>
@@ -91,30 +86,12 @@
     <t>A-&gt;B</t>
   </si>
   <si>
-    <t>BOE</t>
-  </si>
-  <si>
     <t>B-&gt;A</t>
   </si>
   <si>
-    <t>PROM-&gt;AR</t>
-  </si>
-  <si>
     <t>ARE</t>
   </si>
   <si>
-    <t>RAME</t>
-  </si>
-  <si>
-    <t>RAMOE</t>
-  </si>
-  <si>
-    <t>A-&gt;AR</t>
-  </si>
-  <si>
-    <t>B-&gt;AR</t>
-  </si>
-  <si>
     <t>A-&gt;RAM(AR)</t>
   </si>
   <si>
@@ -142,21 +119,12 @@
     <t>MOV A,B</t>
   </si>
   <si>
-    <t>MOV AR,A</t>
-  </si>
-  <si>
-    <t>MOV AR,B</t>
-  </si>
-  <si>
     <t>CLKs</t>
   </si>
   <si>
     <t>JMP val</t>
   </si>
   <si>
-    <t>PROM-&gt;PC</t>
-  </si>
-  <si>
     <t>PCM1</t>
   </si>
   <si>
@@ -172,27 +140,6 @@
     <t>JIN A</t>
   </si>
   <si>
-    <t>(a=0) PROM-&gt;PC</t>
-  </si>
-  <si>
-    <t>PROMAMUX</t>
-  </si>
-  <si>
-    <t>RAMAMUX</t>
-  </si>
-  <si>
-    <t>A-&gt;RAM(addr)</t>
-  </si>
-  <si>
-    <t>B-&gt;RAM(addr)</t>
-  </si>
-  <si>
-    <t>RAM(addr)-&gt;A</t>
-  </si>
-  <si>
-    <t>RAM(addr)-&gt;B</t>
-  </si>
-  <si>
     <t>WR AR,A</t>
   </si>
   <si>
@@ -257,13 +204,190 @@
   </si>
   <si>
     <t>B - 1</t>
+  </si>
+  <si>
+    <t>Sinal</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>BusMux0</t>
+  </si>
+  <si>
+    <t>Data bus multiplexer bit 0</t>
+  </si>
+  <si>
+    <t>BusMux1</t>
+  </si>
+  <si>
+    <t>Data bus multiplexer bit 1</t>
+  </si>
+  <si>
+    <t>AluBMux</t>
+  </si>
+  <si>
+    <t>ALU B Imput Mux control</t>
+  </si>
+  <si>
+    <t>PRomAMux</t>
+  </si>
+  <si>
+    <t>Program ROM Address Mux controls</t>
+  </si>
+  <si>
+    <t>RamAMux</t>
+  </si>
+  <si>
+    <t>RAM address Mux control</t>
+  </si>
+  <si>
+    <t>RamOE</t>
+  </si>
+  <si>
+    <t>RAM Outpur Enable</t>
+  </si>
+  <si>
+    <t>RamE</t>
+  </si>
+  <si>
+    <t>RAM Input Enable</t>
+  </si>
+  <si>
+    <t>ALU opperation select bit 0</t>
+  </si>
+  <si>
+    <t>ALU opperation select bit 1</t>
+  </si>
+  <si>
+    <t>ALU opperation select bit 2</t>
+  </si>
+  <si>
+    <t>ALU opperation select bit 3</t>
+  </si>
+  <si>
+    <t>Program Counter Jump Mode 0</t>
+  </si>
+  <si>
+    <t>Program Counter Jump Mode 1</t>
+  </si>
+  <si>
+    <t>Program Counter Jump Mode 2</t>
+  </si>
+  <si>
+    <t>Clear Instruction Register (zero)</t>
+  </si>
+  <si>
+    <t>INE</t>
+  </si>
+  <si>
+    <t>OUTE</t>
+  </si>
+  <si>
+    <t>Enable Input Registers</t>
+  </si>
+  <si>
+    <t>Enable Output Registers</t>
+  </si>
+  <si>
+    <t>Enable A register</t>
+  </si>
+  <si>
+    <t>AINC</t>
+  </si>
+  <si>
+    <t>Increment A register</t>
+  </si>
+  <si>
+    <t>Enable B register</t>
+  </si>
+  <si>
+    <t>BINC</t>
+  </si>
+  <si>
+    <t>Increment B Register</t>
+  </si>
+  <si>
+    <t>ARINC</t>
+  </si>
+  <si>
+    <t>Increment AR Register</t>
+  </si>
+  <si>
+    <t>Enable AR Register</t>
+  </si>
+  <si>
+    <t>CSET</t>
+  </si>
+  <si>
+    <t>Set Carry Register</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Enable Carry Register</t>
+  </si>
+  <si>
+    <t>CCLR</t>
+  </si>
+  <si>
+    <t>Clear Carry Register</t>
+  </si>
+  <si>
+    <t>Não utilizado</t>
+  </si>
+  <si>
+    <t>Reserva2</t>
+  </si>
+  <si>
+    <t>Reserva1</t>
+  </si>
+  <si>
+    <t>[b7,6]PROM-&gt;AR</t>
+  </si>
+  <si>
+    <t>[b7,6]PROM-&gt;PC</t>
+  </si>
+  <si>
+    <t>(a=0) [b7,6]PROM-&gt;PC</t>
+  </si>
+  <si>
+    <t>A-&gt;RAM([b7,6]PROM)</t>
+  </si>
+  <si>
+    <t>B-&gt;RAM([b7,6]PROM)</t>
+  </si>
+  <si>
+    <t>RAM([b7,6]PROM)-&gt;A</t>
+  </si>
+  <si>
+    <t>RAM([b7,6]PROM)-&gt;B</t>
+  </si>
+  <si>
+    <t>INC A</t>
+  </si>
+  <si>
+    <t>INC B</t>
+  </si>
+  <si>
+    <t>INC AR</t>
+  </si>
+  <si>
+    <t>A+1-&gt;A</t>
+  </si>
+  <si>
+    <t>B+1-&gt;B</t>
+  </si>
+  <si>
+    <t>AR+1-&gt;AR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,8 +401,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,24 +425,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -333,11 +459,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -352,10 +489,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B5E688-C301-4E02-8353-6E2341398D12}">
-  <dimension ref="A1:AA34"/>
+  <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,16 +825,33 @@
     <col min="1" max="1" width="5.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="22" width="6.77734375" style="4" customWidth="1"/>
-    <col min="23" max="23" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="6.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="4" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="5.77734375" style="4" customWidth="1"/>
+    <col min="15" max="18" width="4.5546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="6.109375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="3.5546875" style="4" customWidth="1"/>
+    <col min="23" max="23" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" style="4" customWidth="1"/>
+    <col min="25" max="25" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="8.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="G1" s="4">
         <v>0</v>
       </c>
@@ -751,83 +912,162 @@
       <c r="Z1" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA1" s="4">
+        <v>20</v>
+      </c>
+      <c r="AB1" s="4">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="4">
+        <v>22</v>
+      </c>
+      <c r="AD1" s="4">
+        <v>23</v>
+      </c>
+      <c r="AE1" s="4">
+        <v>24</v>
+      </c>
+      <c r="AF1" s="4">
+        <v>25</v>
+      </c>
+      <c r="AG1" s="4">
+        <v>26</v>
+      </c>
+      <c r="AH1" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="4"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="G2" s="3" t="str">
+        <f>Sinais!$A$2</f>
+        <v>BusMux0</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <f>Sinais!$A$3</f>
+        <v>BusMux1</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>Sinais!$A$4</f>
+        <v>AluBMux</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <f>Sinais!$A$5</f>
+        <v>IRZ</v>
+      </c>
+      <c r="K2" s="6" t="str">
+        <f>Sinais!$A$6</f>
+        <v>PRomAMux</v>
+      </c>
+      <c r="L2" s="6" t="str">
+        <f>Sinais!$A$7</f>
+        <v>RamAMux</v>
+      </c>
+      <c r="M2" s="6" t="str">
+        <f>Sinais!$A$8</f>
+        <v>RamOE</v>
+      </c>
+      <c r="N2" s="6" t="str">
+        <f>Sinais!$A$9</f>
+        <v>RamE</v>
+      </c>
+      <c r="O2" s="3" t="str">
+        <f>Sinais!$A$10</f>
+        <v>OP0</v>
+      </c>
+      <c r="P2" s="3" t="str">
+        <f>Sinais!$A$11</f>
+        <v>OP1</v>
+      </c>
+      <c r="Q2" s="3" t="str">
+        <f>Sinais!$A$12</f>
+        <v>OP2</v>
+      </c>
+      <c r="R2" s="3" t="str">
+        <f>Sinais!$A$13</f>
+        <v>OP3</v>
+      </c>
+      <c r="S2" s="6" t="str">
+        <f>Sinais!$A$14</f>
+        <v>PCM0</v>
+      </c>
+      <c r="T2" s="6" t="str">
+        <f>Sinais!$A$15</f>
+        <v>PCM1</v>
+      </c>
+      <c r="U2" s="6" t="str">
+        <f>Sinais!$A$16</f>
+        <v>PCM2</v>
+      </c>
+      <c r="V2" s="6" t="str">
+        <f>Sinais!$A$17</f>
+        <v>INE</v>
+      </c>
+      <c r="W2" s="3" t="str">
+        <f>Sinais!$A$18</f>
+        <v>OUTE</v>
+      </c>
+      <c r="X2" s="3" t="str">
+        <f>Sinais!$A$19</f>
+        <v>AE</v>
+      </c>
+      <c r="Y2" s="3" t="str">
+        <f>Sinais!$A$20</f>
+        <v>AINC</v>
+      </c>
+      <c r="Z2" s="3" t="str">
+        <f>Sinais!$A$21</f>
+        <v>BE</v>
+      </c>
+      <c r="AA2" s="6" t="str">
+        <f>Sinais!$A$22</f>
+        <v>BINC</v>
+      </c>
+      <c r="AB2" s="6" t="str">
+        <f>Sinais!$A$23</f>
+        <v>ARE</v>
+      </c>
+      <c r="AC2" s="6" t="str">
+        <f>Sinais!$A$24</f>
+        <v>ARINC</v>
+      </c>
+      <c r="AD2" s="6" t="str">
+        <f>Sinais!$A$25</f>
+        <v>CSET</v>
+      </c>
+      <c r="AE2" s="3" t="str">
+        <f>Sinais!$A$26</f>
+        <v>CE</v>
+      </c>
+      <c r="AF2" s="3" t="str">
+        <f>Sinais!$A$27</f>
+        <v>CCLR</v>
+      </c>
+      <c r="AG2" s="3" t="str">
+        <f>Sinais!$A$28</f>
+        <v>Reserva1</v>
+      </c>
+      <c r="AH2" s="3" t="str">
+        <f>Sinais!$A$29</f>
+        <v>Reserva2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -835,18 +1075,18 @@
         <f>DEC2HEX(A3)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="str">
-        <f>"0x"&amp;DEC2HEX(G3*2^0+H3*2^1+I3*2^2+J3*2^3+K3*2^4+L3*2^5+M3*2^6+N3*2^7+O3*2^8+P3*2^9+Q3*2^10+R3*2^11+S3*2^12+T3*2^13+U3*2^14+V3*2^15+W3*2^16+X3*2^17+Y3*2^19+Z3*2^19,5)</f>
-        <v>0x00000</v>
+        <f>"0x"&amp;DEC2HEX(G3*2^0+H3*2^1+I3*2^2+J3*2^3+K3*2^4+L3*2^5+M3*2^6+N3*2^7+O3*2^8+P3*2^9+Q3*2^10+R3*2^11+S3*2^12+T3*2^13+U3*2^14+V3*2^15+W3*2^16+X3*2^17+Y3*2^19+Z3*2^19+AA3*2^20+AB3*2^21+AC3*2^22+AD3*2^23+AE3*2^24+AF3*2^25+AG3*2^26+AH3*2^27,7)</f>
+        <v>0x0000000</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -908,8 +1148,32 @@
       <c r="Z3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -917,33 +1181,33 @@
         <f t="shared" ref="B4:B34" si="0">DEC2HEX(A4)</f>
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>30</v>
+      <c r="C4" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="str">
-        <f t="shared" ref="F4:F34" si="1">"0x"&amp;DEC2HEX(G4*2^0+H4*2^1+I4*2^2+J4*2^3+K4*2^4+L4*2^5+M4*2^6+N4*2^7+O4*2^8+P4*2^9+Q4*2^10+R4*2^11+S4*2^12+T4*2^13+U4*2^14+V4*2^15+W4*2^16+X4*2^17+Y4*2^19+Z4*2^19,5)</f>
-        <v>0x00017</v>
+        <f t="shared" ref="F4:F34" si="1">"0x"&amp;DEC2HEX(G4*2^0+H4*2^1+I4*2^2+J4*2^3+K4*2^4+L4*2^5+M4*2^6+N4*2^7+O4*2^8+P4*2^9+Q4*2^10+R4*2^11+S4*2^12+T4*2^13+U4*2^14+V4*2^15+W4*2^16+X4*2^17+Y4*2^19+Z4*2^19+AA4*2^20+AB4*2^21+AC4*2^22+AD4*2^23+AE4*2^24+AF4*2^25+AG4*2^26+AH4*2^27,7)</f>
+        <v>0x002010A</v>
       </c>
       <c r="G4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
       </c>
       <c r="I4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="2">
         <v>0</v>
@@ -955,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="3">
         <v>0</v>
@@ -982,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4" s="3">
         <v>0</v>
@@ -990,8 +1254,32 @@
       <c r="Z4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -999,30 +1287,30 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>31</v>
+      <c r="C5" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00105</v>
+        <v>0x008000A</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
@@ -1037,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="3">
         <v>0</v>
@@ -1070,10 +1358,34 @@
         <v>0</v>
       </c>
       <c r="Z5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1081,30 +1393,30 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>32</v>
+      <c r="C6" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00405</v>
+        <v>0x020000A</v>
       </c>
       <c r="G6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2">
         <v>0</v>
@@ -1125,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6" s="3">
         <v>0</v>
@@ -1154,8 +1466,32 @@
       <c r="Z6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1163,18 +1499,18 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>33</v>
+      <c r="C7" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00108</v>
+        <v>0x0080000</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -1186,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
@@ -1201,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" s="3">
         <v>0</v>
@@ -1234,10 +1570,34 @@
         <v>0</v>
       </c>
       <c r="Z7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1245,33 +1605,33 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>34</v>
+      <c r="C8" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0x00212</v>
+        <f>"0x"&amp;DEC2HEX(G8*2^0+H8*2^1+I8*2^2+J8*2^3+K8*2^4+L8*2^5+M8*2^6+N8*2^7+O8*2^8+P8*2^9+Q8*2^10+R8*2^11+S8*2^12+T8*2^13+U8*2^14+V8*2^15+W8*2^16+X8*2^17+Y8*2^19+Z8*2^19+AA8*2^20+AB8*2^21+AC8*2^22+AD8*2^23+AE8*2^24+AF8*2^25+AG8*2^26+AH8*2^27,7)</f>
+        <v>0x0020104</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
       </c>
       <c r="H8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="3">
         <v>0</v>
       </c>
       <c r="K8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="2">
         <v>0</v>
@@ -1283,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="O8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="3">
         <v>0</v>
@@ -1310,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="3">
         <v>0</v>
@@ -1318,8 +1678,32 @@
       <c r="Z8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1327,18 +1711,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>35</v>
+      <c r="C9" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0x00408</v>
+        <f>"0x"&amp;DEC2HEX(G9*2^0+H9*2^1+I9*2^2+J9*2^3+K9*2^4+L9*2^5+M9*2^6+N9*2^7+O9*2^8+P9*2^9+Q9*2^10+R9*2^11+S9*2^12+T9*2^13+U9*2^14+V9*2^15+W9*2^16+X9*2^17+Y9*2^19+Z9*2^19+AA9*2^20+AB9*2^21+AC9*2^22+AD9*2^23+AE9*2^24+AF9*2^25+AG9*2^26+AH9*2^27,7)</f>
+        <v>0x0000080</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -1350,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -1362,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="3">
         <v>0</v>
@@ -1371,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" s="3">
         <v>0</v>
@@ -1400,8 +1784,32 @@
       <c r="Z9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1409,33 +1817,33 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>36</v>
+      <c r="C10" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00412</v>
+        <v>0x0000184</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
       </c>
       <c r="H10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="3">
         <v>0</v>
       </c>
       <c r="K10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="2">
         <v>0</v>
@@ -1444,16 +1852,16 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="3">
         <v>0</v>
       </c>
       <c r="Q10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10" s="3">
         <v>0</v>
@@ -1482,8 +1890,32 @@
       <c r="Z10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1491,18 +1923,18 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>52</v>
+      <c r="C11" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00808</v>
+        <v>0x00000A0</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
@@ -1514,19 +1946,19 @@
         <v>0</v>
       </c>
       <c r="J11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="2">
         <v>0</v>
       </c>
       <c r="L11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="2">
         <v>0</v>
       </c>
       <c r="N11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="3">
         <v>0</v>
@@ -1538,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" s="2">
         <v>0</v>
@@ -1564,8 +1996,32 @@
       <c r="Z11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1573,18 +2029,18 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>53</v>
+      <c r="C12" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00A00</v>
+        <v>0x00001A4</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -1593,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="3">
         <v>0</v>
@@ -1602,25 +2058,25 @@
         <v>0</v>
       </c>
       <c r="L12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="2">
         <v>0</v>
       </c>
       <c r="N12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="3">
         <v>0</v>
       </c>
       <c r="R12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="2">
         <v>0</v>
@@ -1646,8 +2102,32 @@
       <c r="Z12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1655,18 +2135,18 @@
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>56</v>
+      <c r="C13" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x1080C</v>
+        <v>0x0000000</v>
       </c>
       <c r="G13" s="3">
         <v>0</v>
@@ -1675,10 +2155,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
@@ -1702,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="2">
         <v>0</v>
@@ -1717,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="W13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X13" s="3">
         <v>0</v>
@@ -1728,8 +2208,32 @@
       <c r="Z13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1737,18 +2241,18 @@
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>57</v>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x10A04</v>
+        <v>0x0000000</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -1757,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="3">
         <v>0</v>
@@ -1778,13 +2282,13 @@
         <v>0</v>
       </c>
       <c r="P14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="3">
         <v>0</v>
       </c>
       <c r="R14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
         <v>0</v>
@@ -1799,7 +2303,7 @@
         <v>0</v>
       </c>
       <c r="W14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="3">
         <v>0</v>
@@ -1810,8 +2314,32 @@
       <c r="Z14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1820,23 +2348,21 @@
         <v>C</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2" t="str">
-        <f t="shared" ref="F15:F18" si="2">"0x"&amp;DEC2HEX(G15*2^0+H15*2^1+I15*2^2+J15*2^3+K15*2^4+L15*2^5+M15*2^6+N15*2^7+O15*2^8+P15*2^9+Q15*2^10+R15*2^11+S15*2^12+T15*2^13+U15*2^14+V15*2^15+W15*2^16+X15*2^17+Y15*2^19+Z15*2^19,5)</f>
-        <v>0x01012</v>
+        <f t="shared" si="1"/>
+        <v>0x0000000</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
       </c>
       <c r="H15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
@@ -1845,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2">
         <v>0</v>
@@ -1869,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="S15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="2">
         <v>0</v>
@@ -1892,8 +2418,32 @@
       <c r="Z15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -1902,17 +2452,15 @@
         <v>D</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0x01110</v>
+        <f t="shared" si="1"/>
+        <v>0x0000000</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
@@ -1926,8 +2474,8 @@
       <c r="J16" s="3">
         <v>0</v>
       </c>
-      <c r="K16" s="5">
-        <v>1</v>
+      <c r="K16" s="2">
+        <v>0</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
@@ -1939,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="3">
         <v>0</v>
@@ -1951,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="S16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="2">
         <v>0</v>
@@ -1974,8 +2522,32 @@
       <c r="Z16" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -1984,17 +2556,15 @@
         <v>E</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="2">
-        <v>2</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="E17" s="2"/>
       <c r="F17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0x00000</v>
+        <f t="shared" si="1"/>
+        <v>0x0000000</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -2056,8 +2626,32 @@
       <c r="Z17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2066,17 +2660,15 @@
         <v>F</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E18" s="2"/>
       <c r="F18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0x00000</v>
+        <f t="shared" si="1"/>
+        <v>0x0000000</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
@@ -2138,8 +2730,32 @@
       <c r="Z18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2148,17 +2764,15 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x02004</v>
+        <v>0x0000000</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
@@ -2167,7 +2781,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="3">
         <v>0</v>
@@ -2200,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19" s="2">
         <v>0</v>
@@ -2220,8 +2834,32 @@
       <c r="Z19" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -2230,17 +2868,15 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="2">
-        <v>2</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E20" s="2"/>
       <c r="F20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x04004</v>
+        <v>0x0000000</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
@@ -2249,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="3">
         <v>0</v>
@@ -2285,7 +2921,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="2">
         <v>0</v>
@@ -2302,8 +2938,32 @@
       <c r="Z20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -2312,13 +2972,15 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2340,8 +3002,32 @@
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -2349,12 +3035,14 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -2376,8 +3064,32 @@
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -2390,7 +3102,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -2412,8 +3124,32 @@
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -2426,7 +3162,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2448,8 +3184,32 @@
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA24" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -2462,7 +3222,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -2484,8 +3244,32 @@
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -2498,7 +3282,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -2520,8 +3304,32 @@
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -2534,7 +3342,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -2556,8 +3364,32 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
@@ -2570,7 +3402,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -2592,8 +3424,32 @@
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
@@ -2606,7 +3462,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -2628,8 +3484,32 @@
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
@@ -2642,7 +3522,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -2664,8 +3544,32 @@
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA30" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
@@ -2678,7 +3582,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2700,8 +3604,32 @@
       <c r="X31" s="3"/>
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
@@ -2714,7 +3642,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2736,8 +3664,32 @@
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
@@ -2750,7 +3702,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -2772,8 +3724,32 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
@@ -2786,7 +3762,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0x00000</v>
+        <v>0x0000000</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -2808,6 +3784,30 @@
       <c r="X34" s="3"/>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
+      <c r="AA34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2816,11 +3816,349 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338D9B5D-04BE-4A6C-9CA6-AB2C6FBF98F6}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3">
+        <v>19</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="2">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="2">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="2">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="3">
+        <v>24</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="3">
+        <v>25</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="3">
+        <v>26</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="3">
+        <v>27</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F822AC2A-DAF4-4305-B498-33A405E08A91}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2832,19 +4170,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2861,7 +4199,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2878,7 +4216,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2895,7 +4233,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2912,7 +4250,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2929,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2946,7 +4284,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2963,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2980,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -2997,7 +4335,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -3013,8 +4351,8 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>73</v>
+      <c r="E11" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -3031,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -3048,7 +4386,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
More instructions added, now with 64 instructions
</commit_message>
<xml_diff>
--- a/docs/sinais.xlsx
+++ b/docs/sinais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\CpuDidatica\CpuDidatica\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0061BE4E-04D3-4439-8B82-4A0E41BA96F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B081785B-9DB6-466A-A927-B9DBB6EC9843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1290" windowWidth="20730" windowHeight="11310" xr2:uid="{18A684C2-09AA-4094-803A-4CBD9ADAA45C}"/>
+    <workbookView xWindow="-20610" yWindow="1290" windowWidth="20730" windowHeight="11040" xr2:uid="{18A684C2-09AA-4094-803A-4CBD9ADAA45C}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="216">
   <si>
     <t>ROM</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>LD B,val</t>
-  </si>
-  <si>
-    <t>LD AR,val</t>
   </si>
   <si>
     <t>MOV B,A</t>
@@ -658,6 +655,39 @@
   </si>
   <si>
     <t>OUT AR+,val</t>
+  </si>
+  <si>
+    <t>LD AR,addr</t>
+  </si>
+  <si>
+    <t>AND A, val</t>
+  </si>
+  <si>
+    <t>XOR A, val</t>
+  </si>
+  <si>
+    <t>ADD A, val</t>
+  </si>
+  <si>
+    <t>SUB A, val</t>
+  </si>
+  <si>
+    <t>A or PROM -&gt; A</t>
+  </si>
+  <si>
+    <t>A and PROM -&gt; A</t>
+  </si>
+  <si>
+    <t>A xor PROM -&gt; A</t>
+  </si>
+  <si>
+    <t>A + PROM -&gt; A</t>
+  </si>
+  <si>
+    <t>A - PROM -&gt; A</t>
+  </si>
+  <si>
+    <t>OR A, val</t>
   </si>
 </sst>
 </file>
@@ -794,7 +824,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -825,6 +854,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,9 +1186,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B5E688-C301-4E02-8353-6E2341398D12}">
   <dimension ref="A1:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,30 +1196,30 @@
     <col min="1" max="1" width="5.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="20" customWidth="1"/>
-    <col min="10" max="10" width="4" style="20" customWidth="1"/>
-    <col min="11" max="11" width="11" style="20" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="7.109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="5.77734375" style="20" customWidth="1"/>
-    <col min="15" max="18" width="4.5546875" style="20" customWidth="1"/>
-    <col min="19" max="21" width="6.109375" style="20" customWidth="1"/>
-    <col min="22" max="22" width="3.5546875" style="20" customWidth="1"/>
-    <col min="23" max="23" width="5.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6" style="20" customWidth="1"/>
-    <col min="25" max="25" width="5.21875" style="21" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.21875" style="21" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="3.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.21875" style="21" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="8.77734375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="19" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="19" customWidth="1"/>
+    <col min="10" max="10" width="4" style="19" customWidth="1"/>
+    <col min="11" max="11" width="11" style="19" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" style="19" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="19" customWidth="1"/>
+    <col min="14" max="14" width="5.77734375" style="19" customWidth="1"/>
+    <col min="15" max="18" width="4.5546875" style="19" customWidth="1"/>
+    <col min="19" max="21" width="6.109375" style="19" customWidth="1"/>
+    <col min="22" max="22" width="3.5546875" style="19" customWidth="1"/>
+    <col min="23" max="23" width="5.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" style="19" customWidth="1"/>
+    <col min="25" max="25" width="5.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="8.77734375" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
@@ -1204,9 +1234,9 @@
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="5" t="str">
@@ -1322,97 +1352,97 @@
         <v>Reserva</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="13" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="16">
-        <v>0</v>
-      </c>
-      <c r="H2" s="16">
-        <v>1</v>
-      </c>
-      <c r="I2" s="16">
+    <row r="2" spans="1:34" s="12" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1</v>
+      </c>
+      <c r="I2" s="15">
         <v>2</v>
       </c>
-      <c r="J2" s="16">
+      <c r="J2" s="15">
         <v>3</v>
       </c>
-      <c r="K2" s="16">
+      <c r="K2" s="15">
         <v>4</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="15">
         <v>5</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="15">
         <v>6</v>
       </c>
-      <c r="N2" s="16">
+      <c r="N2" s="15">
         <v>7</v>
       </c>
-      <c r="O2" s="16">
+      <c r="O2" s="15">
         <v>8</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2" s="15">
         <v>9</v>
       </c>
-      <c r="Q2" s="16">
+      <c r="Q2" s="15">
         <v>10</v>
       </c>
-      <c r="R2" s="16">
+      <c r="R2" s="15">
         <v>11</v>
       </c>
-      <c r="S2" s="16">
+      <c r="S2" s="15">
         <v>12</v>
       </c>
-      <c r="T2" s="16">
+      <c r="T2" s="15">
         <v>13</v>
       </c>
-      <c r="U2" s="16">
+      <c r="U2" s="15">
         <v>14</v>
       </c>
-      <c r="V2" s="16">
+      <c r="V2" s="15">
         <v>15</v>
       </c>
-      <c r="W2" s="16">
+      <c r="W2" s="15">
         <v>16</v>
       </c>
-      <c r="X2" s="16">
+      <c r="X2" s="15">
         <v>17</v>
       </c>
-      <c r="Y2" s="16">
+      <c r="Y2" s="15">
         <v>18</v>
       </c>
-      <c r="Z2" s="16">
+      <c r="Z2" s="15">
         <v>19</v>
       </c>
-      <c r="AA2" s="16">
+      <c r="AA2" s="15">
         <v>20</v>
       </c>
-      <c r="AB2" s="16">
+      <c r="AB2" s="15">
         <v>21</v>
       </c>
-      <c r="AC2" s="16">
+      <c r="AC2" s="15">
         <v>22</v>
       </c>
-      <c r="AD2" s="16">
+      <c r="AD2" s="15">
         <v>23</v>
       </c>
-      <c r="AE2" s="16">
+      <c r="AE2" s="15">
         <v>24</v>
       </c>
-      <c r="AF2" s="16">
+      <c r="AF2" s="15">
         <v>25</v>
       </c>
-      <c r="AG2" s="16">
+      <c r="AG2" s="15">
         <v>26</v>
       </c>
-      <c r="AH2" s="16">
+      <c r="AH2" s="15">
         <v>27</v>
       </c>
     </row>
@@ -1420,11 +1450,11 @@
       <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="str">
+      <c r="B3" s="5" t="str">
         <f>DEC2HEX(A3)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1433,7 +1463,7 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="14" t="str">
+      <c r="F3" s="13" t="str">
         <f>DEC2HEX(G3*2^0+H3*2^1+I3*2^2+J3*2^3+K3*2^4+L3*2^5+M3*2^6+N3*2^7+O3*2^8+P3*2^9+Q3*2^10+R3*2^11+S3*2^12+T3*2^13+U3*2^14+V3*2^15+W3*2^16+X3*2^17+Y3*2^18+Z3*2^19+AA3*2^20+AB3*2^21+AC3*2^22+AD3*2^23+AE3*2^24+AF3*2^25+AG3*2^26+AH3*2^27,7)</f>
         <v>0000000</v>
       </c>
@@ -1526,11 +1556,11 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="str">
+      <c r="B4" s="5" t="str">
         <f t="shared" ref="B4:B66" si="0">DEC2HEX(A4)</f>
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1539,7 +1569,7 @@
       <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="14" t="str">
+      <c r="F4" s="13" t="str">
         <f>DEC2HEX(G4*2^0+H4*2^1+I4*2^2+J4*2^3+K4*2^4+L4*2^5+M4*2^6+N4*2^7+O4*2^8+P4*2^9+Q4*2^10+R4*2^11+S4*2^12+T4*2^13+U4*2^14+V4*2^15+W4*2^16+X4*2^17+Y4*2^18+Z4*2^19+AA4*2^20+AB4*2^21+AC4*2^22+AD4*2^23+AE4*2^24+AF4*2^25+AG4*2^26+AH4*2^27,7)</f>
         <v>002010A</v>
       </c>
@@ -1632,11 +1662,11 @@
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="str">
+      <c r="B5" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1645,7 +1675,7 @@
       <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="14" t="str">
+      <c r="F5" s="13" t="str">
         <f t="shared" ref="F5:F66" si="1">DEC2HEX(G5*2^0+H5*2^1+I5*2^2+J5*2^3+K5*2^4+L5*2^5+M5*2^6+N5*2^7+O5*2^8+P5*2^9+Q5*2^10+R5*2^11+S5*2^12+T5*2^13+U5*2^14+V5*2^15+W5*2^16+X5*2^17+Y5*2^18+Z5*2^19+AA5*2^20+AB5*2^21+AC5*2^22+AD5*2^23+AE5*2^24+AF5*2^25+AG5*2^26+AH5*2^27,7)</f>
         <v>008000A</v>
       </c>
@@ -1738,20 +1768,20 @@
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="str">
+      <c r="B6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>24</v>
+      <c r="C6" s="22" t="s">
+        <v>205</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
       </c>
-      <c r="F6" s="14" t="str">
+      <c r="F6" s="13" t="str">
         <f t="shared" si="1"/>
         <v>020000A</v>
       </c>
@@ -1844,20 +1874,20 @@
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="str">
+      <c r="B7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>124</v>
+      <c r="C7" s="22" t="s">
+        <v>123</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="14" t="str">
+      <c r="F7" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0020112</v>
       </c>
@@ -1950,20 +1980,20 @@
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="str">
+      <c r="B8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>125</v>
+      <c r="C8" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" s="14" t="str">
+      <c r="F8" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0080012</v>
       </c>
@@ -2056,20 +2086,20 @@
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="B9" s="5" t="str">
+        <f>DEC2HEX(A9)</f>
         <v>6</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>184</v>
+      <c r="C9" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="14" t="str">
+      <c r="F9" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0420112</v>
       </c>
@@ -2162,20 +2192,20 @@
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="str">
+      <c r="B10" s="5" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>185</v>
+      <c r="C10" s="22" t="s">
+        <v>184</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="14" t="str">
+      <c r="F10" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0480012</v>
       </c>
@@ -2268,12 +2298,12 @@
       <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="str">
+      <c r="B11" s="5" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>25</v>
+      <c r="C11" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
@@ -2281,7 +2311,7 @@
       <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" s="14" t="str">
+      <c r="F11" s="13" t="str">
         <f>DEC2HEX(G11*2^0+H11*2^1+I11*2^2+J11*2^3+K11*2^4+L11*2^5+M11*2^6+N11*2^7+O11*2^8+P11*2^9+Q11*2^10+R11*2^11+S11*2^12+T11*2^13+U11*2^14+V11*2^15+W11*2^16+X11*2^17+Y11*2^18+Z11*2^19+AA11*2^20+AB11*2^21+AC11*2^22+AD11*2^23+AE11*2^24+AF11*2^25+AG11*2^26+AH11*2^27,7)</f>
         <v>0080000</v>
       </c>
@@ -2374,12 +2404,12 @@
       <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="str">
+      <c r="B12" s="5" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>26</v>
+      <c r="C12" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>16</v>
@@ -2387,7 +2417,7 @@
       <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="14" t="str">
+      <c r="F12" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0020104</v>
       </c>
@@ -2480,12 +2510,12 @@
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="str">
+      <c r="B13" s="5" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>31</v>
+      <c r="C13" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>18</v>
@@ -2493,7 +2523,7 @@
       <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="14" t="str">
+      <c r="F13" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0000080</v>
       </c>
@@ -2586,12 +2616,12 @@
       <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="str">
+      <c r="B14" s="5" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>32</v>
+      <c r="C14" s="22" t="s">
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>19</v>
@@ -2599,7 +2629,7 @@
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="14" t="str">
+      <c r="F14" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0000184</v>
       </c>
@@ -2692,20 +2722,20 @@
       <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="str">
+      <c r="B15" s="5" t="str">
         <f t="shared" si="0"/>
         <v>C</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>188</v>
+      <c r="C15" s="22" t="s">
+        <v>187</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="2">
         <v>1</v>
       </c>
-      <c r="F15" s="14" t="str">
+      <c r="F15" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0400080</v>
       </c>
@@ -2798,20 +2828,20 @@
       <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="2" t="str">
+      <c r="B16" s="5" t="str">
         <f t="shared" si="0"/>
         <v>D</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>189</v>
+      <c r="C16" s="22" t="s">
+        <v>188</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
       </c>
-      <c r="F16" s="14" t="str">
+      <c r="F16" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0400184</v>
       </c>
@@ -2904,20 +2934,20 @@
       <c r="A17" s="2">
         <v>14</v>
       </c>
-      <c r="B17" s="2" t="str">
+      <c r="B17" s="5" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>35</v>
+      <c r="C17" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
       </c>
-      <c r="F17" s="14" t="str">
+      <c r="F17" s="13" t="str">
         <f t="shared" si="1"/>
         <v>00000A8</v>
       </c>
@@ -3010,20 +3040,20 @@
       <c r="A18" s="2">
         <v>15</v>
       </c>
-      <c r="B18" s="2" t="str">
+      <c r="B18" s="5" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>36</v>
+      <c r="C18" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E18" s="2">
         <v>2</v>
       </c>
-      <c r="F18" s="14" t="str">
+      <c r="F18" s="13" t="str">
         <f t="shared" si="1"/>
         <v>00001AC</v>
       </c>
@@ -3116,12 +3146,12 @@
       <c r="A19" s="2">
         <v>16</v>
       </c>
-      <c r="B19" s="2" t="str">
+      <c r="B19" s="5" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>33</v>
+      <c r="C19" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>20</v>
@@ -3129,7 +3159,7 @@
       <c r="E19" s="2">
         <v>1</v>
       </c>
-      <c r="F19" s="14" t="str">
+      <c r="F19" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0020143</v>
       </c>
@@ -3222,12 +3252,12 @@
       <c r="A20" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="2" t="str">
+      <c r="B20" s="5" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>34</v>
+      <c r="C20" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>21</v>
@@ -3235,7 +3265,7 @@
       <c r="E20" s="2">
         <v>1</v>
       </c>
-      <c r="F20" s="14" t="str">
+      <c r="F20" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0080043</v>
       </c>
@@ -3328,20 +3358,20 @@
       <c r="A21" s="2">
         <v>18</v>
       </c>
-      <c r="B21" s="2" t="str">
+      <c r="B21" s="5" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>190</v>
+      <c r="C21" s="22" t="s">
+        <v>189</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
       </c>
-      <c r="F21" s="14" t="str">
+      <c r="F21" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0420143</v>
       </c>
@@ -3434,20 +3464,20 @@
       <c r="A22" s="2">
         <v>19</v>
       </c>
-      <c r="B22" s="2" t="str">
+      <c r="B22" s="5" t="str">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>191</v>
+      <c r="C22" s="22" t="s">
+        <v>190</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
       </c>
-      <c r="F22" s="14" t="str">
+      <c r="F22" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0480043</v>
       </c>
@@ -3540,20 +3570,20 @@
       <c r="A23" s="2">
         <v>20</v>
       </c>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="5" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>37</v>
+      <c r="C23" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E23" s="2">
         <v>2</v>
       </c>
-      <c r="F23" s="14" t="str">
+      <c r="F23" s="13" t="str">
         <f t="shared" si="1"/>
         <v>002016B</v>
       </c>
@@ -3646,20 +3676,20 @@
       <c r="A24" s="2">
         <v>21</v>
       </c>
-      <c r="B24" s="2" t="str">
+      <c r="B24" s="5" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>38</v>
+      <c r="C24" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" s="2">
         <v>2</v>
       </c>
-      <c r="F24" s="14" t="str">
+      <c r="F24" s="13" t="str">
         <f t="shared" si="1"/>
         <v>008006B</v>
       </c>
@@ -3752,20 +3782,20 @@
       <c r="A25" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="2" t="str">
+      <c r="B25" s="5" t="str">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>120</v>
+      <c r="C25" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
       </c>
-      <c r="F25" s="14" t="str">
+      <c r="F25" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0028101</v>
       </c>
@@ -3858,20 +3888,20 @@
       <c r="A26" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="2" t="str">
+      <c r="B26" s="5" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>121</v>
+      <c r="C26" s="22" t="s">
+        <v>120</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
       </c>
-      <c r="F26" s="14" t="str">
+      <c r="F26" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0088001</v>
       </c>
@@ -3964,20 +3994,20 @@
       <c r="A27" s="2">
         <v>24</v>
       </c>
-      <c r="B27" s="2" t="str">
+      <c r="B27" s="5" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>196</v>
+      <c r="C27" s="22" t="s">
+        <v>195</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
       </c>
-      <c r="F27" s="14" t="str">
+      <c r="F27" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0428101</v>
       </c>
@@ -4070,20 +4100,20 @@
       <c r="A28" s="2">
         <v>25</v>
       </c>
-      <c r="B28" s="2" t="str">
+      <c r="B28" s="5" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>197</v>
+      <c r="C28" s="22" t="s">
+        <v>196</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
       </c>
-      <c r="F28" s="14" t="str">
+      <c r="F28" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0488001</v>
       </c>
@@ -4176,20 +4206,20 @@
       <c r="A29" s="2">
         <v>26</v>
       </c>
-      <c r="B29" s="2" t="str">
+      <c r="B29" s="5" t="str">
         <f t="shared" si="0"/>
         <v>1A</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>122</v>
+      <c r="C29" s="22" t="s">
+        <v>121</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" s="2">
         <v>2</v>
       </c>
-      <c r="F29" s="14" t="str">
+      <c r="F29" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0028129</v>
       </c>
@@ -4282,20 +4312,20 @@
       <c r="A30" s="2">
         <v>27</v>
       </c>
-      <c r="B30" s="2" t="str">
+      <c r="B30" s="5" t="str">
         <f>DEC2HEX(A30)</f>
         <v>1B</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>123</v>
+      <c r="C30" s="22" t="s">
+        <v>122</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
       </c>
-      <c r="F30" s="14" t="str">
+      <c r="F30" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0088029</v>
       </c>
@@ -4388,20 +4418,20 @@
       <c r="A31" s="2">
         <v>28</v>
       </c>
-      <c r="B31" s="2" t="str">
+      <c r="B31" s="5" t="str">
         <f t="shared" si="0"/>
         <v>1C</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>116</v>
+      <c r="C31" s="22" t="s">
+        <v>115</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
       </c>
-      <c r="F31" s="14" t="str">
+      <c r="F31" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0010000</v>
       </c>
@@ -4494,20 +4524,20 @@
       <c r="A32" s="2">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="str">
+      <c r="B32" s="5" t="str">
         <f t="shared" si="0"/>
         <v>1D</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>117</v>
+      <c r="C32" s="22" t="s">
+        <v>116</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
       </c>
-      <c r="F32" s="14" t="str">
+      <c r="F32" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0010104</v>
       </c>
@@ -4600,20 +4630,20 @@
       <c r="A33" s="2">
         <v>30</v>
       </c>
-      <c r="B33" s="2" t="str">
+      <c r="B33" s="5" t="str">
         <f t="shared" si="0"/>
         <v>1E</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="E33" s="5">
         <v>2</v>
       </c>
-      <c r="F33" s="14" t="str">
+      <c r="F33" s="13" t="str">
         <f t="shared" si="1"/>
         <v>001000A</v>
       </c>
@@ -4706,20 +4736,20 @@
       <c r="A34" s="2">
         <v>31</v>
       </c>
-      <c r="B34" s="2" t="str">
+      <c r="B34" s="5" t="str">
         <f t="shared" si="0"/>
         <v>1F</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>201</v>
-      </c>
       <c r="E34" s="2">
         <v>1</v>
       </c>
-      <c r="F34" s="14" t="str">
+      <c r="F34" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0410000</v>
       </c>
@@ -4812,20 +4842,20 @@
       <c r="A35" s="2">
         <v>32</v>
       </c>
-      <c r="B35" s="2" t="str">
+      <c r="B35" s="5" t="str">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>204</v>
+      <c r="C35" s="22" t="s">
+        <v>203</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E35" s="2">
         <v>1</v>
       </c>
-      <c r="F35" s="14" t="str">
+      <c r="F35" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0410104</v>
       </c>
@@ -4918,20 +4948,20 @@
       <c r="A36" s="2">
         <v>33</v>
       </c>
-      <c r="B36" s="2" t="str">
+      <c r="B36" s="5" t="str">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>205</v>
+      <c r="C36" s="22" t="s">
+        <v>204</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="E36" s="2">
+        <v>202</v>
+      </c>
+      <c r="E36" s="5">
         <v>2</v>
       </c>
-      <c r="F36" s="14" t="str">
+      <c r="F36" s="13" t="str">
         <f t="shared" si="1"/>
         <v>041000A</v>
       </c>
@@ -5024,20 +5054,20 @@
       <c r="A37" s="2">
         <v>34</v>
       </c>
-      <c r="B37" s="2" t="str">
+      <c r="B37" s="5" t="str">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="2">
+      <c r="C37" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="5">
         <v>2</v>
       </c>
-      <c r="F37" s="14" t="str">
+      <c r="F37" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0010028</v>
       </c>
@@ -5130,20 +5160,20 @@
       <c r="A38" s="2">
         <v>35</v>
       </c>
-      <c r="B38" s="2" t="str">
+      <c r="B38" s="5" t="str">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E38" s="2">
+      <c r="C38" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="5">
         <v>2</v>
       </c>
-      <c r="F38" s="14" t="str">
+      <c r="F38" s="13" t="str">
         <f t="shared" si="1"/>
         <v>001012C</v>
       </c>
@@ -5236,20 +5266,20 @@
       <c r="A39" s="2">
         <v>36</v>
       </c>
-      <c r="B39" s="2" t="str">
+      <c r="B39" s="5" t="str">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>103</v>
+      <c r="C39" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E39" s="2">
         <v>1</v>
       </c>
-      <c r="F39" s="14" t="str">
+      <c r="F39" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0040000</v>
       </c>
@@ -5342,20 +5372,20 @@
       <c r="A40" s="2">
         <v>37</v>
       </c>
-      <c r="B40" s="2" t="str">
+      <c r="B40" s="5" t="str">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>104</v>
+      <c r="C40" s="22" t="s">
+        <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E40" s="2">
         <v>1</v>
       </c>
-      <c r="F40" s="14" t="str">
+      <c r="F40" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0100000</v>
       </c>
@@ -5448,20 +5478,20 @@
       <c r="A41" s="2">
         <v>38</v>
       </c>
-      <c r="B41" s="2" t="str">
+      <c r="B41" s="5" t="str">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>105</v>
+      <c r="C41" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E41" s="2">
         <v>1</v>
       </c>
-      <c r="F41" s="14" t="str">
+      <c r="F41" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0400000</v>
       </c>
@@ -5554,20 +5584,20 @@
       <c r="A42" s="2">
         <v>39</v>
       </c>
-      <c r="B42" s="2" t="str">
+      <c r="B42" s="5" t="str">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E42" s="2">
+      <c r="C42" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="5">
         <v>2</v>
       </c>
-      <c r="F42" s="14" t="str">
+      <c r="F42" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0001008</v>
       </c>
@@ -5660,20 +5690,20 @@
       <c r="A43" s="2">
         <v>40</v>
       </c>
-      <c r="B43" s="2" t="str">
+      <c r="B43" s="5" t="str">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E43" s="2">
+      <c r="C43" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="5">
         <v>2</v>
       </c>
-      <c r="F43" s="14" t="str">
+      <c r="F43" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0002008</v>
       </c>
@@ -5766,20 +5796,20 @@
       <c r="A44" s="2">
         <v>41</v>
       </c>
-      <c r="B44" s="2" t="str">
+      <c r="B44" s="5" t="str">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E44" s="2">
+      <c r="C44" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="5">
         <v>2</v>
       </c>
-      <c r="F44" s="14" t="str">
+      <c r="F44" s="13" t="str">
         <f t="shared" si="1"/>
         <v>000300C</v>
       </c>
@@ -5872,20 +5902,20 @@
       <c r="A45" s="2">
         <v>42</v>
       </c>
-      <c r="B45" s="2" t="str">
+      <c r="B45" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2A</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E45" s="2">
+      <c r="C45" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" s="5">
         <v>2</v>
       </c>
-      <c r="F45" s="14" t="str">
+      <c r="F45" s="13" t="str">
         <f t="shared" si="1"/>
         <v>000400C</v>
       </c>
@@ -5978,20 +6008,20 @@
       <c r="A46" s="2">
         <v>43</v>
       </c>
-      <c r="B46" s="2" t="str">
+      <c r="B46" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2B</v>
       </c>
-      <c r="C46" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" s="2">
+      <c r="C46" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46" s="5">
         <v>2</v>
       </c>
-      <c r="F46" s="14" t="str">
+      <c r="F46" s="13" t="str">
         <f t="shared" si="1"/>
         <v>000500C</v>
       </c>
@@ -6084,20 +6114,20 @@
       <c r="A47" s="2">
         <v>44</v>
       </c>
-      <c r="B47" s="2" t="str">
+      <c r="B47" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2C</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E47" s="2">
+      <c r="C47" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E47" s="5">
         <v>2</v>
       </c>
-      <c r="F47" s="14" t="str">
+      <c r="F47" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0006008</v>
       </c>
@@ -6190,20 +6220,20 @@
       <c r="A48" s="2">
         <v>45</v>
       </c>
-      <c r="B48" s="2" t="str">
+      <c r="B48" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2D</v>
       </c>
-      <c r="C48" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" s="2">
+      <c r="C48" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="5">
         <v>2</v>
       </c>
-      <c r="F48" s="14" t="str">
+      <c r="F48" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0007008</v>
       </c>
@@ -6296,20 +6326,20 @@
       <c r="A49" s="2">
         <v>46</v>
       </c>
-      <c r="B49" s="2" t="str">
+      <c r="B49" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2E</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>144</v>
+      <c r="C49" s="22" t="s">
+        <v>143</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E49" s="2">
         <v>1</v>
       </c>
-      <c r="F49" s="14" t="str">
+      <c r="F49" s="13" t="str">
         <f t="shared" si="1"/>
         <v>1800000</v>
       </c>
@@ -6402,20 +6432,20 @@
       <c r="A50" s="2">
         <v>47</v>
       </c>
-      <c r="B50" s="2" t="str">
+      <c r="B50" s="5" t="str">
         <f t="shared" si="0"/>
         <v>2F</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>145</v>
+      <c r="C50" s="22" t="s">
+        <v>144</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E50" s="2">
         <v>1</v>
       </c>
-      <c r="F50" s="14" t="str">
+      <c r="F50" s="13" t="str">
         <f t="shared" si="1"/>
         <v>3000000</v>
       </c>
@@ -6508,20 +6538,20 @@
       <c r="A51" s="2">
         <v>48</v>
       </c>
-      <c r="B51" s="2" t="str">
+      <c r="B51" s="5" t="str">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>42</v>
+      <c r="C51" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E51" s="2">
         <v>1</v>
       </c>
-      <c r="F51" s="14" t="str">
+      <c r="F51" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0020200</v>
       </c>
@@ -6614,20 +6644,20 @@
       <c r="A52" s="2">
         <v>49</v>
       </c>
-      <c r="B52" s="2" t="str">
+      <c r="B52" s="5" t="str">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>157</v>
+      <c r="C52" s="22" t="s">
+        <v>156</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E52" s="2">
         <v>1</v>
       </c>
-      <c r="F52" s="14" t="str">
+      <c r="F52" s="13" t="str">
         <f t="shared" si="1"/>
         <v>0020304</v>
       </c>
@@ -6720,34 +6750,34 @@
       <c r="A53" s="2">
         <v>50</v>
       </c>
-      <c r="B53" s="2" t="str">
+      <c r="B53" s="5" t="str">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>158</v>
+      <c r="C53" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="E53" s="2">
-        <v>1</v>
-      </c>
-      <c r="F53" s="14" t="str">
+        <v>2</v>
+      </c>
+      <c r="F53" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0020404</v>
+        <v>002030A</v>
       </c>
       <c r="G53" s="5">
         <v>0</v>
       </c>
       <c r="H53" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" s="5">
         <v>0</v>
@@ -6762,13 +6792,13 @@
         <v>0</v>
       </c>
       <c r="O53" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P53" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q53" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R53" s="5">
         <v>0</v>
@@ -6826,22 +6856,22 @@
       <c r="A54" s="2">
         <v>51</v>
       </c>
-      <c r="B54" s="2" t="str">
+      <c r="B54" s="5" t="str">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>159</v>
+      <c r="C54" s="22" t="s">
+        <v>157</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E54" s="2">
         <v>1</v>
       </c>
-      <c r="F54" s="14" t="str">
+      <c r="F54" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0020504</v>
+        <v>0020404</v>
       </c>
       <c r="G54" s="5">
         <v>0</v>
@@ -6868,7 +6898,7 @@
         <v>0</v>
       </c>
       <c r="O54" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P54" s="5">
         <v>0</v>
@@ -6932,34 +6962,34 @@
       <c r="A55" s="2">
         <v>52</v>
       </c>
-      <c r="B55" s="2" t="str">
+      <c r="B55" s="5" t="str">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>160</v>
+      <c r="C55" s="22" t="s">
+        <v>206</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="E55" s="2">
-        <v>1</v>
-      </c>
-      <c r="F55" s="14" t="str">
+        <v>2</v>
+      </c>
+      <c r="F55" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1020604</v>
+        <v>002040A</v>
       </c>
       <c r="G55" s="5">
         <v>0</v>
       </c>
       <c r="H55" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K55" s="5">
         <v>0</v>
@@ -6977,7 +7007,7 @@
         <v>0</v>
       </c>
       <c r="P55" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q55" s="5">
         <v>1</v>
@@ -7022,7 +7052,7 @@
         <v>0</v>
       </c>
       <c r="AE55" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF55" s="5">
         <v>0</v>
@@ -7038,22 +7068,22 @@
       <c r="A56" s="2">
         <v>53</v>
       </c>
-      <c r="B56" s="2" t="str">
+      <c r="B56" s="5" t="str">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="C56" s="10" t="s">
-        <v>161</v>
+      <c r="C56" s="22" t="s">
+        <v>158</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E56" s="2">
         <v>1</v>
       </c>
-      <c r="F56" s="14" t="str">
+      <c r="F56" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1020704</v>
+        <v>0020504</v>
       </c>
       <c r="G56" s="5">
         <v>0</v>
@@ -7083,7 +7113,7 @@
         <v>1</v>
       </c>
       <c r="P56" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q56" s="5">
         <v>1</v>
@@ -7128,7 +7158,7 @@
         <v>0</v>
       </c>
       <c r="AE56" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF56" s="5">
         <v>0</v>
@@ -7144,34 +7174,34 @@
       <c r="A57" s="2">
         <v>54</v>
       </c>
-      <c r="B57" s="2" t="str">
+      <c r="B57" s="5" t="str">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>162</v>
+      <c r="C57" s="22" t="s">
+        <v>207</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>154</v>
+        <v>212</v>
       </c>
       <c r="E57" s="2">
-        <v>1</v>
-      </c>
-      <c r="F57" s="14" t="str">
+        <v>2</v>
+      </c>
+      <c r="F57" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1020800</v>
+        <v>002050A</v>
       </c>
       <c r="G57" s="5">
         <v>0</v>
       </c>
       <c r="H57" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="5">
         <v>0</v>
       </c>
       <c r="J57" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K57" s="5">
         <v>0</v>
@@ -7186,16 +7216,16 @@
         <v>0</v>
       </c>
       <c r="O57" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P57" s="5">
         <v>0</v>
       </c>
       <c r="Q57" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R57" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S57" s="5">
         <v>0</v>
@@ -7234,7 +7264,7 @@
         <v>0</v>
       </c>
       <c r="AE57" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF57" s="5">
         <v>0</v>
@@ -7250,22 +7280,22 @@
       <c r="A58" s="2">
         <v>55</v>
       </c>
-      <c r="B58" s="2" t="str">
+      <c r="B58" s="5" t="str">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="C58" s="10" t="s">
-        <v>163</v>
+      <c r="C58" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E58" s="2">
         <v>1</v>
       </c>
-      <c r="F58" s="14" t="str">
+      <c r="F58" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1080904</v>
+        <v>1020604</v>
       </c>
       <c r="G58" s="5">
         <v>0</v>
@@ -7292,16 +7322,16 @@
         <v>0</v>
       </c>
       <c r="O58" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P58" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q58" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R58" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S58" s="5">
         <v>0</v>
@@ -7319,13 +7349,13 @@
         <v>0</v>
       </c>
       <c r="X58" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y58" s="5">
         <v>0</v>
       </c>
       <c r="Z58" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA58" s="5">
         <v>0</v>
@@ -7356,34 +7386,34 @@
       <c r="A59" s="2">
         <v>56</v>
       </c>
-      <c r="B59" s="2" t="str">
+      <c r="B59" s="5" t="str">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="C59" s="10" t="s">
-        <v>164</v>
+      <c r="C59" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>166</v>
+        <v>213</v>
       </c>
       <c r="E59" s="2">
-        <v>1</v>
-      </c>
-      <c r="F59" s="14" t="str">
+        <v>2</v>
+      </c>
+      <c r="F59" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1020A00</v>
+        <v>102060A</v>
       </c>
       <c r="G59" s="5">
         <v>0</v>
       </c>
       <c r="H59" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" s="5">
         <v>0</v>
       </c>
       <c r="J59" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" s="5">
         <v>0</v>
@@ -7404,10 +7434,10 @@
         <v>1</v>
       </c>
       <c r="Q59" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R59" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S59" s="5">
         <v>0</v>
@@ -7462,22 +7492,22 @@
       <c r="A60" s="2">
         <v>57</v>
       </c>
-      <c r="B60" s="2" t="str">
+      <c r="B60" s="5" t="str">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="C60" s="10" t="s">
-        <v>165</v>
+      <c r="C60" s="22" t="s">
+        <v>160</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="E60" s="2">
         <v>1</v>
       </c>
-      <c r="F60" s="14" t="str">
+      <c r="F60" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>1020B00</v>
+        <v>1020704</v>
       </c>
       <c r="G60" s="5">
         <v>0</v>
@@ -7486,7 +7516,7 @@
         <v>0</v>
       </c>
       <c r="I60" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" s="5">
         <v>0</v>
@@ -7510,10 +7540,10 @@
         <v>1</v>
       </c>
       <c r="Q60" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R60" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S60" s="5">
         <v>0</v>
@@ -7568,34 +7598,34 @@
       <c r="A61" s="2">
         <v>58</v>
       </c>
-      <c r="B61" s="2" t="str">
+      <c r="B61" s="5" t="str">
         <f t="shared" si="0"/>
         <v>3A</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>178</v>
+      <c r="C61" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="E61" s="2">
-        <v>1</v>
-      </c>
-      <c r="F61" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>40A0000</v>
+        <v>2</v>
+      </c>
+      <c r="F61" s="13" t="str">
+        <f t="shared" ref="F61:F66" si="2">DEC2HEX(G61*2^0+H61*2^1+I61*2^2+J61*2^3+K61*2^4+L61*2^5+M61*2^6+N61*2^7+O61*2^8+P61*2^9+Q61*2^10+R61*2^11+S61*2^12+T61*2^13+U61*2^14+V61*2^15+W61*2^16+X61*2^17+Y61*2^18+Z61*2^19+AA61*2^20+AB61*2^21+AC61*2^22+AD61*2^23+AE61*2^24+AF61*2^25+AG61*2^26+AH61*2^27,7)</f>
+        <v>102070A</v>
       </c>
       <c r="G61" s="5">
         <v>0</v>
       </c>
       <c r="H61" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" s="5">
         <v>0</v>
       </c>
       <c r="J61" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K61" s="5">
         <v>0</v>
@@ -7610,13 +7640,13 @@
         <v>0</v>
       </c>
       <c r="O61" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P61" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q61" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R61" s="5">
         <v>0</v>
@@ -7643,7 +7673,7 @@
         <v>0</v>
       </c>
       <c r="Z61" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA61" s="5">
         <v>0</v>
@@ -7658,13 +7688,13 @@
         <v>0</v>
       </c>
       <c r="AE61" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF61" s="5">
         <v>0</v>
       </c>
       <c r="AG61" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH61" s="5">
         <v>0</v>
@@ -7678,41 +7708,103 @@
         <f t="shared" si="0"/>
         <v>3B</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>0000000</v>
-      </c>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
-      <c r="P62" s="5"/>
-      <c r="Q62" s="5"/>
-      <c r="R62" s="5"/>
-      <c r="S62" s="5"/>
-      <c r="T62" s="5"/>
-      <c r="U62" s="5"/>
-      <c r="V62" s="5"/>
-      <c r="W62" s="5"/>
-      <c r="X62" s="5"/>
-      <c r="Y62" s="5"/>
-      <c r="Z62" s="5"/>
-      <c r="AA62" s="5"/>
-      <c r="AB62" s="5"/>
-      <c r="AC62" s="5"/>
-      <c r="AD62" s="5"/>
-      <c r="AE62" s="5"/>
-      <c r="AF62" s="5"/>
-      <c r="AG62" s="5"/>
-      <c r="AH62" s="5"/>
+      <c r="C62" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1</v>
+      </c>
+      <c r="F62" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>1020800</v>
+      </c>
+      <c r="G62" s="5">
+        <v>0</v>
+      </c>
+      <c r="H62" s="5">
+        <v>0</v>
+      </c>
+      <c r="I62" s="5">
+        <v>0</v>
+      </c>
+      <c r="J62" s="5">
+        <v>0</v>
+      </c>
+      <c r="K62" s="5">
+        <v>0</v>
+      </c>
+      <c r="L62" s="5">
+        <v>0</v>
+      </c>
+      <c r="M62" s="5">
+        <v>0</v>
+      </c>
+      <c r="N62" s="5">
+        <v>0</v>
+      </c>
+      <c r="O62" s="5">
+        <v>0</v>
+      </c>
+      <c r="P62" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="5">
+        <v>0</v>
+      </c>
+      <c r="R62" s="5">
+        <v>1</v>
+      </c>
+      <c r="S62" s="5">
+        <v>0</v>
+      </c>
+      <c r="T62" s="5">
+        <v>0</v>
+      </c>
+      <c r="U62" s="5">
+        <v>0</v>
+      </c>
+      <c r="V62" s="5">
+        <v>0</v>
+      </c>
+      <c r="W62" s="5">
+        <v>0</v>
+      </c>
+      <c r="X62" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y62" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE62" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG62" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH62" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
@@ -7722,41 +7814,103 @@
         <f t="shared" si="0"/>
         <v>3C</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>0000000</v>
-      </c>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
-      <c r="P63" s="5"/>
-      <c r="Q63" s="5"/>
-      <c r="R63" s="5"/>
-      <c r="S63" s="5"/>
-      <c r="T63" s="5"/>
-      <c r="U63" s="5"/>
-      <c r="V63" s="5"/>
-      <c r="W63" s="5"/>
-      <c r="X63" s="5"/>
-      <c r="Y63" s="5"/>
-      <c r="Z63" s="5"/>
-      <c r="AA63" s="5"/>
-      <c r="AB63" s="5"/>
-      <c r="AC63" s="5"/>
-      <c r="AD63" s="5"/>
-      <c r="AE63" s="5"/>
-      <c r="AF63" s="5"/>
-      <c r="AG63" s="5"/>
-      <c r="AH63" s="5"/>
+      <c r="C63" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1</v>
+      </c>
+      <c r="F63" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>1080904</v>
+      </c>
+      <c r="G63" s="5">
+        <v>0</v>
+      </c>
+      <c r="H63" s="5">
+        <v>0</v>
+      </c>
+      <c r="I63" s="5">
+        <v>1</v>
+      </c>
+      <c r="J63" s="5">
+        <v>0</v>
+      </c>
+      <c r="K63" s="5">
+        <v>0</v>
+      </c>
+      <c r="L63" s="5">
+        <v>0</v>
+      </c>
+      <c r="M63" s="5">
+        <v>0</v>
+      </c>
+      <c r="N63" s="5">
+        <v>0</v>
+      </c>
+      <c r="O63" s="5">
+        <v>1</v>
+      </c>
+      <c r="P63" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="5">
+        <v>0</v>
+      </c>
+      <c r="R63" s="5">
+        <v>1</v>
+      </c>
+      <c r="S63" s="5">
+        <v>0</v>
+      </c>
+      <c r="T63" s="5">
+        <v>0</v>
+      </c>
+      <c r="U63" s="5">
+        <v>0</v>
+      </c>
+      <c r="V63" s="5">
+        <v>0</v>
+      </c>
+      <c r="W63" s="5">
+        <v>0</v>
+      </c>
+      <c r="X63" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y63" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z63" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE63" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG63" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH63" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
@@ -7766,41 +7920,103 @@
         <f t="shared" si="0"/>
         <v>3D</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>0000000</v>
-      </c>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="5"/>
-      <c r="R64" s="5"/>
-      <c r="S64" s="5"/>
-      <c r="T64" s="5"/>
-      <c r="U64" s="5"/>
-      <c r="V64" s="5"/>
-      <c r="W64" s="5"/>
-      <c r="X64" s="5"/>
-      <c r="Y64" s="5"/>
-      <c r="Z64" s="5"/>
-      <c r="AA64" s="5"/>
-      <c r="AB64" s="5"/>
-      <c r="AC64" s="5"/>
-      <c r="AD64" s="5"/>
-      <c r="AE64" s="5"/>
-      <c r="AF64" s="5"/>
-      <c r="AG64" s="5"/>
-      <c r="AH64" s="5"/>
+      <c r="C64" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E64" s="2">
+        <v>1</v>
+      </c>
+      <c r="F64" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>1020A00</v>
+      </c>
+      <c r="G64" s="5">
+        <v>0</v>
+      </c>
+      <c r="H64" s="5">
+        <v>0</v>
+      </c>
+      <c r="I64" s="5">
+        <v>0</v>
+      </c>
+      <c r="J64" s="5">
+        <v>0</v>
+      </c>
+      <c r="K64" s="5">
+        <v>0</v>
+      </c>
+      <c r="L64" s="5">
+        <v>0</v>
+      </c>
+      <c r="M64" s="5">
+        <v>0</v>
+      </c>
+      <c r="N64" s="5">
+        <v>0</v>
+      </c>
+      <c r="O64" s="5">
+        <v>0</v>
+      </c>
+      <c r="P64" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="5">
+        <v>0</v>
+      </c>
+      <c r="R64" s="5">
+        <v>1</v>
+      </c>
+      <c r="S64" s="5">
+        <v>0</v>
+      </c>
+      <c r="T64" s="5">
+        <v>0</v>
+      </c>
+      <c r="U64" s="5">
+        <v>0</v>
+      </c>
+      <c r="V64" s="5">
+        <v>0</v>
+      </c>
+      <c r="W64" s="5">
+        <v>0</v>
+      </c>
+      <c r="X64" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y64" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE64" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH64" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
@@ -7810,41 +8026,103 @@
         <f t="shared" si="0"/>
         <v>3E</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>0000000</v>
-      </c>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
-      <c r="P65" s="5"/>
-      <c r="Q65" s="5"/>
-      <c r="R65" s="5"/>
-      <c r="S65" s="5"/>
-      <c r="T65" s="5"/>
-      <c r="U65" s="5"/>
-      <c r="V65" s="5"/>
-      <c r="W65" s="5"/>
-      <c r="X65" s="5"/>
-      <c r="Y65" s="5"/>
-      <c r="Z65" s="5"/>
-      <c r="AA65" s="5"/>
-      <c r="AB65" s="5"/>
-      <c r="AC65" s="5"/>
-      <c r="AD65" s="5"/>
-      <c r="AE65" s="5"/>
-      <c r="AF65" s="5"/>
-      <c r="AG65" s="5"/>
-      <c r="AH65" s="5"/>
+      <c r="C65" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E65" s="2">
+        <v>1</v>
+      </c>
+      <c r="F65" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>1020B00</v>
+      </c>
+      <c r="G65" s="5">
+        <v>0</v>
+      </c>
+      <c r="H65" s="5">
+        <v>0</v>
+      </c>
+      <c r="I65" s="5">
+        <v>0</v>
+      </c>
+      <c r="J65" s="5">
+        <v>0</v>
+      </c>
+      <c r="K65" s="5">
+        <v>0</v>
+      </c>
+      <c r="L65" s="5">
+        <v>0</v>
+      </c>
+      <c r="M65" s="5">
+        <v>0</v>
+      </c>
+      <c r="N65" s="5">
+        <v>0</v>
+      </c>
+      <c r="O65" s="5">
+        <v>1</v>
+      </c>
+      <c r="P65" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="5">
+        <v>0</v>
+      </c>
+      <c r="R65" s="5">
+        <v>1</v>
+      </c>
+      <c r="S65" s="5">
+        <v>0</v>
+      </c>
+      <c r="T65" s="5">
+        <v>0</v>
+      </c>
+      <c r="U65" s="5">
+        <v>0</v>
+      </c>
+      <c r="V65" s="5">
+        <v>0</v>
+      </c>
+      <c r="W65" s="5">
+        <v>0</v>
+      </c>
+      <c r="X65" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y65" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE65" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG65" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH65" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
@@ -7854,41 +8132,103 @@
         <f t="shared" si="0"/>
         <v>3F</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>0000000</v>
-      </c>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
-      <c r="M66" s="5"/>
-      <c r="N66" s="5"/>
-      <c r="O66" s="5"/>
-      <c r="P66" s="5"/>
-      <c r="Q66" s="5"/>
-      <c r="R66" s="5"/>
-      <c r="S66" s="5"/>
-      <c r="T66" s="5"/>
-      <c r="U66" s="5"/>
-      <c r="V66" s="5"/>
-      <c r="W66" s="5"/>
-      <c r="X66" s="5"/>
-      <c r="Y66" s="5"/>
-      <c r="Z66" s="5"/>
-      <c r="AA66" s="5"/>
-      <c r="AB66" s="5"/>
-      <c r="AC66" s="5"/>
-      <c r="AD66" s="5"/>
-      <c r="AE66" s="5"/>
-      <c r="AF66" s="5"/>
-      <c r="AG66" s="5"/>
-      <c r="AH66" s="5"/>
+      <c r="C66" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E66" s="2">
+        <v>1</v>
+      </c>
+      <c r="F66" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>40A0000</v>
+      </c>
+      <c r="G66" s="5">
+        <v>0</v>
+      </c>
+      <c r="H66" s="5">
+        <v>0</v>
+      </c>
+      <c r="I66" s="5">
+        <v>0</v>
+      </c>
+      <c r="J66" s="5">
+        <v>0</v>
+      </c>
+      <c r="K66" s="5">
+        <v>0</v>
+      </c>
+      <c r="L66" s="5">
+        <v>0</v>
+      </c>
+      <c r="M66" s="5">
+        <v>0</v>
+      </c>
+      <c r="N66" s="5">
+        <v>0</v>
+      </c>
+      <c r="O66" s="5">
+        <v>0</v>
+      </c>
+      <c r="P66" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="5">
+        <v>0</v>
+      </c>
+      <c r="R66" s="5">
+        <v>0</v>
+      </c>
+      <c r="S66" s="5">
+        <v>0</v>
+      </c>
+      <c r="T66" s="5">
+        <v>0</v>
+      </c>
+      <c r="U66" s="5">
+        <v>0</v>
+      </c>
+      <c r="V66" s="5">
+        <v>0</v>
+      </c>
+      <c r="W66" s="5">
+        <v>0</v>
+      </c>
+      <c r="X66" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y66" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA66" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB66" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC66" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD66" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE66" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF66" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG66" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH66" s="5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7944,44 +8284,44 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -7992,51 +8332,51 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -8047,7 +8387,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -8058,7 +8398,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -8069,7 +8409,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -8080,62 +8420,62 @@
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="3">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -8146,18 +8486,18 @@
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="3">
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -8168,18 +8508,18 @@
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2">
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -8190,73 +8530,73 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="2">
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="2">
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="3">
         <v>24</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B27" s="3">
         <v>25</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B28" s="3">
         <v>26</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B29" s="3">
         <v>27</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -8294,7 +8634,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -8310,8 +8650,8 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>40</v>
+      <c r="E2" s="21" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -8327,8 +8667,8 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>41</v>
+      <c r="E3" s="21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -8344,8 +8684,8 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>42</v>
+      <c r="E4" s="21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -8361,8 +8701,8 @@
       <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>43</v>
+      <c r="E5" s="21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -8378,8 +8718,8 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>44</v>
+      <c r="E6" s="21" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -8395,8 +8735,8 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>45</v>
+      <c r="E7" s="21" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -8412,8 +8752,8 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>46</v>
+      <c r="E8" s="21" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -8429,8 +8769,8 @@
       <c r="D9" s="2">
         <v>1</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>47</v>
+      <c r="E9" s="21" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -8446,8 +8786,8 @@
       <c r="D10" s="2">
         <v>0</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>48</v>
+      <c r="E10" s="21" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -8463,8 +8803,8 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>51</v>
+      <c r="E11" s="21" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -8480,8 +8820,8 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>49</v>
+      <c r="E12" s="21" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -8497,8 +8837,8 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>50</v>
+      <c r="E13" s="21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -8577,28 +8917,28 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53.109375" customWidth="1"/>
-    <col min="2" max="2" width="10" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>183</v>
+      <c r="D1" s="17" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="8">
         <v>3</v>
@@ -8608,7 +8948,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -8618,7 +8958,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
@@ -8628,7 +8968,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="8">
         <v>2</v>
@@ -8652,7 +8992,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="8">
         <v>4</v>
@@ -8662,7 +9002,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="8">
         <v>5</v>
@@ -8672,7 +9012,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="8">
         <v>3</v>
@@ -8761,7 +9101,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -8773,15 +9113,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09ED8AC-4881-4758-87A3-A9237751EEC8}">
   <dimension ref="A1:A65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A65" sqref="A1:A65"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection sqref="A1:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -9087,85 +9427,85 @@
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f>Instruções!F53</f>
-        <v>0020404</v>
+        <v>002030A</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f>Instruções!F54</f>
-        <v>0020504</v>
+        <v>0020404</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f>Instruções!F55</f>
-        <v>1020604</v>
+        <v>002040A</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f>Instruções!F56</f>
-        <v>1020704</v>
+        <v>0020504</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f>Instruções!F57</f>
-        <v>1020800</v>
+        <v>002050A</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
         <f>Instruções!F58</f>
-        <v>1080904</v>
+        <v>1020604</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
         <f>Instruções!F59</f>
-        <v>1020A00</v>
+        <v>102060A</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
         <f>Instruções!F60</f>
-        <v>1020B00</v>
+        <v>1020704</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
         <f>Instruções!F61</f>
-        <v>40A0000</v>
+        <v>102070A</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
         <f>Instruções!F62</f>
-        <v>0000000</v>
+        <v>1020800</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
         <f>Instruções!F63</f>
-        <v>0000000</v>
+        <v>1080904</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
         <f>Instruções!F64</f>
-        <v>0000000</v>
+        <v>1020A00</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
         <f>Instruções!F65</f>
-        <v>0000000</v>
+        <v>1020B00</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="str">
         <f>Instruções!F66</f>
-        <v>0000000</v>
+        <v>40A0000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>